<commit_message>
Betters for la porra
</commit_message>
<xml_diff>
--- a/laporra/XXX_NoHay2Sin3_WC2022.xlsx
+++ b/laporra/XXX_NoHay2Sin3_WC2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolasy/Developer/nicoyuste/www.nicoyuste.es/laporra/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589215A9-3F32-1541-8971-E67BF4BBBD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7BB354-E9A2-1C43-A68A-1EF185D973EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19340" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{4CA72BBF-35EA-F240-BA10-523169D3F12A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{4CA72BBF-35EA-F240-BA10-523169D3F12A}"/>
   </bookViews>
   <sheets>
     <sheet name="INICIO" sheetId="5" r:id="rId1"/>
@@ -1874,105 +1874,23 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="28" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="16" fontId="8" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2046,23 +1964,105 @@
     <xf numFmtId="0" fontId="8" fillId="25" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="16" fontId="8" fillId="28" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="16" fontId="8" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2072,7 +2072,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="64">
@@ -3133,7 +3133,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3505,7 +3505,7 @@
   <dimension ref="B3:Q906"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3560,7 +3560,7 @@
       </c>
     </row>
     <row r="4" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="193" t="s">
+      <c r="B4" s="232" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="32"/>
@@ -3583,17 +3583,17 @@
         <f t="shared" ref="J4:J35" si="1">IF(OR(ISBLANK($F4),ISBLANK($G4)),"-",IF(F4&lt;G4,3,IF(F4&gt;G4,0,1)))</f>
         <v>-</v>
       </c>
-      <c r="L4" s="178" t="s">
+      <c r="L4" s="217" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="179"/>
-      <c r="N4" s="179"/>
-      <c r="O4" s="179"/>
-      <c r="P4" s="179"/>
-      <c r="Q4" s="180"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="218"/>
+      <c r="Q4" s="219"/>
     </row>
     <row r="5" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="194"/>
+      <c r="B5" s="233"/>
       <c r="C5" s="6"/>
       <c r="D5" s="49" t="s">
         <v>39</v>
@@ -3634,7 +3634,7 @@
       </c>
     </row>
     <row r="6" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="194"/>
+      <c r="B6" s="233"/>
       <c r="C6" s="6"/>
       <c r="D6" s="49" t="s">
         <v>40</v>
@@ -3680,7 +3680,7 @@
       </c>
     </row>
     <row r="7" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="194"/>
+      <c r="B7" s="233"/>
       <c r="C7" s="6"/>
       <c r="D7" s="49" t="s">
         <v>40</v>
@@ -3726,7 +3726,7 @@
       </c>
     </row>
     <row r="8" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="194"/>
+      <c r="B8" s="233"/>
       <c r="C8" s="6"/>
       <c r="D8" s="49" t="s">
         <v>41</v>
@@ -3772,7 +3772,7 @@
       </c>
     </row>
     <row r="9" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="195"/>
+      <c r="B9" s="234"/>
       <c r="C9" s="35"/>
       <c r="D9" s="50" t="s">
         <v>41</v>
@@ -3851,7 +3851,7 @@
       </c>
     </row>
     <row r="12" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="181" t="s">
+      <c r="B12" s="220" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="20"/>
@@ -3874,17 +3874,17 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L12" s="184" t="s">
+      <c r="L12" s="223" t="s">
         <v>30</v>
       </c>
-      <c r="M12" s="185"/>
-      <c r="N12" s="185"/>
-      <c r="O12" s="185"/>
-      <c r="P12" s="185"/>
-      <c r="Q12" s="186"/>
+      <c r="M12" s="224"/>
+      <c r="N12" s="224"/>
+      <c r="O12" s="224"/>
+      <c r="P12" s="224"/>
+      <c r="Q12" s="225"/>
     </row>
     <row r="13" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="182"/>
+      <c r="B13" s="221"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16" t="s">
         <v>39</v>
@@ -3925,7 +3925,7 @@
       </c>
     </row>
     <row r="14" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="182"/>
+      <c r="B14" s="221"/>
       <c r="C14" s="16"/>
       <c r="D14" s="16" t="s">
         <v>40</v>
@@ -3971,7 +3971,7 @@
       </c>
     </row>
     <row r="15" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="182"/>
+      <c r="B15" s="221"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16" t="s">
         <v>40</v>
@@ -4017,7 +4017,7 @@
       </c>
     </row>
     <row r="16" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="182"/>
+      <c r="B16" s="221"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16" t="s">
         <v>41</v>
@@ -4063,7 +4063,7 @@
       </c>
     </row>
     <row r="17" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="183"/>
+      <c r="B17" s="222"/>
       <c r="C17" s="23"/>
       <c r="D17" s="23" t="s">
         <v>41</v>
@@ -4142,7 +4142,7 @@
       </c>
     </row>
     <row r="20" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="226" t="s">
         <v>43</v>
       </c>
       <c r="C20" s="51"/>
@@ -4165,17 +4165,17 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L20" s="190" t="s">
+      <c r="L20" s="229" t="s">
         <v>53</v>
       </c>
-      <c r="M20" s="191"/>
-      <c r="N20" s="191"/>
-      <c r="O20" s="191"/>
-      <c r="P20" s="191"/>
-      <c r="Q20" s="192"/>
+      <c r="M20" s="230"/>
+      <c r="N20" s="230"/>
+      <c r="O20" s="230"/>
+      <c r="P20" s="230"/>
+      <c r="Q20" s="231"/>
     </row>
     <row r="21" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="188"/>
+      <c r="B21" s="227"/>
       <c r="C21" s="164"/>
       <c r="D21" s="164" t="s">
         <v>39</v>
@@ -4216,7 +4216,7 @@
       </c>
     </row>
     <row r="22" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="188"/>
+      <c r="B22" s="227"/>
       <c r="C22" s="164"/>
       <c r="D22" s="164" t="s">
         <v>40</v>
@@ -4262,7 +4262,7 @@
       </c>
     </row>
     <row r="23" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="188"/>
+      <c r="B23" s="227"/>
       <c r="C23" s="164"/>
       <c r="D23" s="164" t="s">
         <v>40</v>
@@ -4308,7 +4308,7 @@
       </c>
     </row>
     <row r="24" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="188"/>
+      <c r="B24" s="227"/>
       <c r="C24" s="164"/>
       <c r="D24" s="164" t="s">
         <v>41</v>
@@ -4354,7 +4354,7 @@
       </c>
     </row>
     <row r="25" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="189"/>
+      <c r="B25" s="228"/>
       <c r="C25" s="54"/>
       <c r="D25" s="54" t="s">
         <v>41</v>
@@ -4433,7 +4433,7 @@
       </c>
     </row>
     <row r="28" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="196" t="s">
+      <c r="B28" s="235" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="135"/>
@@ -4456,17 +4456,17 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-      <c r="L28" s="175" t="s">
+      <c r="L28" s="214" t="s">
         <v>58</v>
       </c>
-      <c r="M28" s="176"/>
-      <c r="N28" s="176"/>
-      <c r="O28" s="176"/>
-      <c r="P28" s="176"/>
-      <c r="Q28" s="177"/>
+      <c r="M28" s="215"/>
+      <c r="N28" s="215"/>
+      <c r="O28" s="215"/>
+      <c r="P28" s="215"/>
+      <c r="Q28" s="216"/>
     </row>
     <row r="29" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="197"/>
+      <c r="B29" s="236"/>
       <c r="C29" s="161"/>
       <c r="D29" s="161" t="s">
         <v>39</v>
@@ -4507,7 +4507,7 @@
       </c>
     </row>
     <row r="30" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="197"/>
+      <c r="B30" s="236"/>
       <c r="C30" s="161"/>
       <c r="D30" s="161" t="s">
         <v>40</v>
@@ -4553,7 +4553,7 @@
       </c>
     </row>
     <row r="31" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="197"/>
+      <c r="B31" s="236"/>
       <c r="C31" s="161"/>
       <c r="D31" s="161" t="s">
         <v>40</v>
@@ -4599,7 +4599,7 @@
       </c>
     </row>
     <row r="32" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="197"/>
+      <c r="B32" s="236"/>
       <c r="C32" s="161"/>
       <c r="D32" s="161" t="s">
         <v>41</v>
@@ -4645,7 +4645,7 @@
       </c>
     </row>
     <row r="33" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="198"/>
+      <c r="B33" s="237"/>
       <c r="C33" s="138"/>
       <c r="D33" s="138" t="s">
         <v>41</v>
@@ -4728,7 +4728,7 @@
       </c>
     </row>
     <row r="36" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="220" t="s">
+      <c r="B36" s="193" t="s">
         <v>49</v>
       </c>
       <c r="C36" s="65"/>
@@ -4751,17 +4751,17 @@
         <f t="shared" ref="J36:J68" si="3">IF(OR(ISBLANK($F36),ISBLANK($G36)),"-",IF(F36&lt;G36,3,IF(F36&gt;G36,0,1)))</f>
         <v>-</v>
       </c>
-      <c r="L36" s="208" t="s">
+      <c r="L36" s="181" t="s">
         <v>57</v>
       </c>
-      <c r="M36" s="209"/>
-      <c r="N36" s="209"/>
-      <c r="O36" s="209"/>
-      <c r="P36" s="209"/>
-      <c r="Q36" s="210"/>
+      <c r="M36" s="182"/>
+      <c r="N36" s="182"/>
+      <c r="O36" s="182"/>
+      <c r="P36" s="182"/>
+      <c r="Q36" s="183"/>
     </row>
     <row r="37" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="221"/>
+      <c r="B37" s="194"/>
       <c r="C37" s="157"/>
       <c r="D37" s="157" t="s">
         <v>39</v>
@@ -4802,7 +4802,7 @@
       </c>
     </row>
     <row r="38" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="221"/>
+      <c r="B38" s="194"/>
       <c r="C38" s="157"/>
       <c r="D38" s="157" t="s">
         <v>40</v>
@@ -4848,7 +4848,7 @@
       </c>
     </row>
     <row r="39" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="221"/>
+      <c r="B39" s="194"/>
       <c r="C39" s="157"/>
       <c r="D39" s="157" t="s">
         <v>40</v>
@@ -4894,7 +4894,7 @@
       </c>
     </row>
     <row r="40" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="221"/>
+      <c r="B40" s="194"/>
       <c r="C40" s="157"/>
       <c r="D40" s="157" t="s">
         <v>41</v>
@@ -4940,7 +4940,7 @@
       </c>
     </row>
     <row r="41" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="222"/>
+      <c r="B41" s="195"/>
       <c r="C41" s="68"/>
       <c r="D41" s="68" t="s">
         <v>41</v>
@@ -5019,7 +5019,7 @@
       </c>
     </row>
     <row r="44" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="223" t="s">
+      <c r="B44" s="196" t="s">
         <v>50</v>
       </c>
       <c r="C44" s="78"/>
@@ -5042,17 +5042,17 @@
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="L44" s="211" t="s">
+      <c r="L44" s="184" t="s">
         <v>56</v>
       </c>
-      <c r="M44" s="212"/>
-      <c r="N44" s="212"/>
-      <c r="O44" s="212"/>
-      <c r="P44" s="212"/>
-      <c r="Q44" s="213"/>
+      <c r="M44" s="185"/>
+      <c r="N44" s="185"/>
+      <c r="O44" s="185"/>
+      <c r="P44" s="185"/>
+      <c r="Q44" s="186"/>
     </row>
     <row r="45" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="224"/>
+      <c r="B45" s="197"/>
       <c r="C45" s="77"/>
       <c r="D45" s="77" t="s">
         <v>39</v>
@@ -5093,7 +5093,7 @@
       </c>
     </row>
     <row r="46" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="224"/>
+      <c r="B46" s="197"/>
       <c r="C46" s="77"/>
       <c r="D46" s="77" t="s">
         <v>40</v>
@@ -5139,7 +5139,7 @@
       </c>
     </row>
     <row r="47" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="224"/>
+      <c r="B47" s="197"/>
       <c r="C47" s="77"/>
       <c r="D47" s="77" t="s">
         <v>40</v>
@@ -5185,7 +5185,7 @@
       </c>
     </row>
     <row r="48" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="224"/>
+      <c r="B48" s="197"/>
       <c r="C48" s="77"/>
       <c r="D48" s="77" t="s">
         <v>41</v>
@@ -5231,7 +5231,7 @@
       </c>
     </row>
     <row r="49" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="225"/>
+      <c r="B49" s="198"/>
       <c r="C49" s="81"/>
       <c r="D49" s="81" t="s">
         <v>41</v>
@@ -5310,7 +5310,7 @@
       </c>
     </row>
     <row r="52" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="226" t="s">
+      <c r="B52" s="199" t="s">
         <v>51</v>
       </c>
       <c r="C52" s="91"/>
@@ -5333,17 +5333,17 @@
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="L52" s="214" t="s">
+      <c r="L52" s="187" t="s">
         <v>55</v>
       </c>
-      <c r="M52" s="215"/>
-      <c r="N52" s="215"/>
-      <c r="O52" s="215"/>
-      <c r="P52" s="215"/>
-      <c r="Q52" s="216"/>
+      <c r="M52" s="188"/>
+      <c r="N52" s="188"/>
+      <c r="O52" s="188"/>
+      <c r="P52" s="188"/>
+      <c r="Q52" s="189"/>
     </row>
     <row r="53" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="227"/>
+      <c r="B53" s="200"/>
       <c r="C53" s="90"/>
       <c r="D53" s="90" t="s">
         <v>39</v>
@@ -5384,7 +5384,7 @@
       </c>
     </row>
     <row r="54" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="227"/>
+      <c r="B54" s="200"/>
       <c r="C54" s="90"/>
       <c r="D54" s="90" t="s">
         <v>40</v>
@@ -5430,7 +5430,7 @@
       </c>
     </row>
     <row r="55" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B55" s="227"/>
+      <c r="B55" s="200"/>
       <c r="C55" s="90"/>
       <c r="D55" s="90" t="s">
         <v>40</v>
@@ -5476,7 +5476,7 @@
       </c>
     </row>
     <row r="56" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="227"/>
+      <c r="B56" s="200"/>
       <c r="C56" s="90"/>
       <c r="D56" s="90" t="s">
         <v>41</v>
@@ -5522,7 +5522,7 @@
       </c>
     </row>
     <row r="57" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="228"/>
+      <c r="B57" s="201"/>
       <c r="C57" s="94"/>
       <c r="D57" s="94" t="s">
         <v>41</v>
@@ -5601,7 +5601,7 @@
       </c>
     </row>
     <row r="60" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="229" t="s">
+      <c r="B60" s="202" t="s">
         <v>52</v>
       </c>
       <c r="C60" s="104"/>
@@ -5624,17 +5624,17 @@
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="L60" s="217" t="s">
+      <c r="L60" s="190" t="s">
         <v>54</v>
       </c>
-      <c r="M60" s="218"/>
-      <c r="N60" s="218"/>
-      <c r="O60" s="218"/>
-      <c r="P60" s="218"/>
-      <c r="Q60" s="219"/>
+      <c r="M60" s="191"/>
+      <c r="N60" s="191"/>
+      <c r="O60" s="191"/>
+      <c r="P60" s="191"/>
+      <c r="Q60" s="192"/>
     </row>
     <row r="61" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="230"/>
+      <c r="B61" s="203"/>
       <c r="C61" s="103"/>
       <c r="D61" s="103" t="s">
         <v>39</v>
@@ -5675,7 +5675,7 @@
       </c>
     </row>
     <row r="62" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="230"/>
+      <c r="B62" s="203"/>
       <c r="C62" s="103"/>
       <c r="D62" s="103" t="s">
         <v>40</v>
@@ -5721,7 +5721,7 @@
       </c>
     </row>
     <row r="63" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="230"/>
+      <c r="B63" s="203"/>
       <c r="C63" s="103"/>
       <c r="D63" s="103" t="s">
         <v>40</v>
@@ -5767,7 +5767,7 @@
       </c>
     </row>
     <row r="64" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="230"/>
+      <c r="B64" s="203"/>
       <c r="C64" s="103"/>
       <c r="D64" s="103" t="s">
         <v>41</v>
@@ -5813,7 +5813,7 @@
       </c>
     </row>
     <row r="65" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="231"/>
+      <c r="B65" s="204"/>
       <c r="C65" s="107"/>
       <c r="D65" s="107" t="s">
         <v>41</v>
@@ -5886,12 +5886,12 @@
       <c r="C68" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E68" s="200" t="s">
+      <c r="E68" s="206" t="s">
         <v>79</v>
       </c>
-      <c r="F68" s="200"/>
-      <c r="G68" s="200"/>
-      <c r="H68" s="200"/>
+      <c r="F68" s="206"/>
+      <c r="G68" s="206"/>
+      <c r="H68" s="206"/>
       <c r="I68" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -5902,7 +5902,7 @@
       </c>
     </row>
     <row r="69" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="204" t="s">
+      <c r="B69" s="210" t="s">
         <v>80</v>
       </c>
       <c r="C69" s="116"/>
@@ -5924,18 +5924,18 @@
         <v>-</v>
       </c>
       <c r="J69" s="5"/>
-      <c r="L69" s="232" t="str">
+      <c r="L69" s="179" t="str">
         <f t="shared" ref="L69:L76" si="4">IF(I69=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M69" s="233"/>
-      <c r="N69" s="233"/>
-      <c r="O69" s="233"/>
-      <c r="P69" s="233"/>
+      <c r="M69" s="180"/>
+      <c r="N69" s="180"/>
+      <c r="O69" s="180"/>
+      <c r="P69" s="180"/>
       <c r="Q69" s="170"/>
     </row>
     <row r="70" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="205"/>
+      <c r="B70" s="211"/>
       <c r="C70" s="122"/>
       <c r="D70" s="122" t="s">
         <v>87</v>
@@ -5955,18 +5955,18 @@
         <v>-</v>
       </c>
       <c r="J70" s="5"/>
-      <c r="L70" s="234" t="str">
+      <c r="L70" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M70" s="235"/>
-      <c r="N70" s="235"/>
-      <c r="O70" s="235"/>
-      <c r="P70" s="235"/>
+      <c r="M70" s="176"/>
+      <c r="N70" s="176"/>
+      <c r="O70" s="176"/>
+      <c r="P70" s="176"/>
       <c r="Q70" s="171"/>
     </row>
     <row r="71" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="205"/>
+      <c r="B71" s="211"/>
       <c r="C71" s="122"/>
       <c r="D71" s="122" t="s">
         <v>88</v>
@@ -5986,18 +5986,18 @@
         <v>-</v>
       </c>
       <c r="J71" s="5"/>
-      <c r="L71" s="234" t="str">
+      <c r="L71" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M71" s="235"/>
-      <c r="N71" s="235"/>
-      <c r="O71" s="235"/>
-      <c r="P71" s="235"/>
+      <c r="M71" s="176"/>
+      <c r="N71" s="176"/>
+      <c r="O71" s="176"/>
+      <c r="P71" s="176"/>
       <c r="Q71" s="171"/>
     </row>
     <row r="72" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="206"/>
+      <c r="B72" s="212"/>
       <c r="C72" s="122"/>
       <c r="D72" s="122" t="s">
         <v>89</v>
@@ -6017,18 +6017,18 @@
         <v>-</v>
       </c>
       <c r="J72" s="5"/>
-      <c r="L72" s="234" t="str">
+      <c r="L72" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M72" s="235"/>
-      <c r="N72" s="235"/>
-      <c r="O72" s="235"/>
-      <c r="P72" s="235"/>
+      <c r="M72" s="176"/>
+      <c r="N72" s="176"/>
+      <c r="O72" s="176"/>
+      <c r="P72" s="176"/>
       <c r="Q72" s="171"/>
     </row>
     <row r="73" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="206"/>
+      <c r="B73" s="212"/>
       <c r="C73" s="122"/>
       <c r="D73" s="122" t="s">
         <v>90</v>
@@ -6048,18 +6048,18 @@
         <v>-</v>
       </c>
       <c r="J73" s="5"/>
-      <c r="L73" s="234" t="str">
+      <c r="L73" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M73" s="235"/>
-      <c r="N73" s="235"/>
-      <c r="O73" s="235"/>
-      <c r="P73" s="235"/>
+      <c r="M73" s="176"/>
+      <c r="N73" s="176"/>
+      <c r="O73" s="176"/>
+      <c r="P73" s="176"/>
       <c r="Q73" s="171"/>
     </row>
     <row r="74" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="206"/>
+      <c r="B74" s="212"/>
       <c r="C74" s="122"/>
       <c r="D74" s="122" t="s">
         <v>91</v>
@@ -6079,18 +6079,18 @@
         <v>-</v>
       </c>
       <c r="J74" s="5"/>
-      <c r="L74" s="234" t="str">
+      <c r="L74" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M74" s="235"/>
-      <c r="N74" s="235"/>
-      <c r="O74" s="235"/>
-      <c r="P74" s="235"/>
+      <c r="M74" s="176"/>
+      <c r="N74" s="176"/>
+      <c r="O74" s="176"/>
+      <c r="P74" s="176"/>
       <c r="Q74" s="171"/>
     </row>
     <row r="75" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="206"/>
+      <c r="B75" s="212"/>
       <c r="C75" s="122"/>
       <c r="D75" s="122" t="s">
         <v>92</v>
@@ -6110,18 +6110,18 @@
         <v>-</v>
       </c>
       <c r="J75" s="5"/>
-      <c r="L75" s="234" t="str">
+      <c r="L75" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M75" s="235"/>
-      <c r="N75" s="235"/>
-      <c r="O75" s="235"/>
-      <c r="P75" s="235"/>
+      <c r="M75" s="176"/>
+      <c r="N75" s="176"/>
+      <c r="O75" s="176"/>
+      <c r="P75" s="176"/>
       <c r="Q75" s="171"/>
     </row>
     <row r="76" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="207"/>
+      <c r="B76" s="213"/>
       <c r="C76" s="119"/>
       <c r="D76" s="119" t="s">
         <v>93</v>
@@ -6141,14 +6141,14 @@
         <v>-</v>
       </c>
       <c r="J76" s="5"/>
-      <c r="L76" s="234" t="str">
+      <c r="L76" s="175" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M76" s="235"/>
-      <c r="N76" s="235"/>
-      <c r="O76" s="235"/>
-      <c r="P76" s="235"/>
+      <c r="M76" s="176"/>
+      <c r="N76" s="176"/>
+      <c r="O76" s="176"/>
+      <c r="P76" s="176"/>
       <c r="Q76" s="171"/>
     </row>
     <row r="77" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6165,12 +6165,12 @@
       <c r="C78" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E78" s="200" t="s">
+      <c r="E78" s="206" t="s">
         <v>81</v>
       </c>
-      <c r="F78" s="200"/>
-      <c r="G78" s="200"/>
-      <c r="H78" s="200"/>
+      <c r="F78" s="206"/>
+      <c r="G78" s="206"/>
+      <c r="H78" s="206"/>
       <c r="L78" s="167"/>
       <c r="M78" s="168"/>
       <c r="N78" s="168"/>
@@ -6179,7 +6179,7 @@
       <c r="Q78" s="169"/>
     </row>
     <row r="79" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="204" t="s">
+      <c r="B79" s="210" t="s">
         <v>84</v>
       </c>
       <c r="C79" s="116"/>
@@ -6201,18 +6201,18 @@
         <v>-</v>
       </c>
       <c r="J79" s="5"/>
-      <c r="L79" s="234" t="str">
+      <c r="L79" s="175" t="str">
         <f>IF(I79=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M79" s="235"/>
-      <c r="N79" s="235"/>
-      <c r="O79" s="235"/>
-      <c r="P79" s="235"/>
+      <c r="M79" s="176"/>
+      <c r="N79" s="176"/>
+      <c r="O79" s="176"/>
+      <c r="P79" s="176"/>
       <c r="Q79" s="171"/>
     </row>
     <row r="80" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="206"/>
+      <c r="B80" s="212"/>
       <c r="C80" s="122"/>
       <c r="D80" s="122" t="s">
         <v>95</v>
@@ -6232,18 +6232,18 @@
         <v>-</v>
       </c>
       <c r="J80" s="5"/>
-      <c r="L80" s="234" t="str">
+      <c r="L80" s="175" t="str">
         <f>IF(I80=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M80" s="235"/>
-      <c r="N80" s="235"/>
-      <c r="O80" s="235"/>
-      <c r="P80" s="235"/>
+      <c r="M80" s="176"/>
+      <c r="N80" s="176"/>
+      <c r="O80" s="176"/>
+      <c r="P80" s="176"/>
       <c r="Q80" s="171"/>
     </row>
     <row r="81" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="206"/>
+      <c r="B81" s="212"/>
       <c r="C81" s="122"/>
       <c r="D81" s="122" t="s">
         <v>96</v>
@@ -6263,18 +6263,18 @@
         <v>-</v>
       </c>
       <c r="J81" s="5"/>
-      <c r="L81" s="234" t="str">
+      <c r="L81" s="175" t="str">
         <f>IF(I81=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M81" s="235"/>
-      <c r="N81" s="235"/>
-      <c r="O81" s="235"/>
-      <c r="P81" s="235"/>
+      <c r="M81" s="176"/>
+      <c r="N81" s="176"/>
+      <c r="O81" s="176"/>
+      <c r="P81" s="176"/>
       <c r="Q81" s="171"/>
     </row>
     <row r="82" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="207"/>
+      <c r="B82" s="213"/>
       <c r="C82" s="119"/>
       <c r="D82" s="119" t="s">
         <v>97</v>
@@ -6294,14 +6294,14 @@
         <v>-</v>
       </c>
       <c r="J82" s="5"/>
-      <c r="L82" s="234" t="str">
+      <c r="L82" s="175" t="str">
         <f>IF(I82=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M82" s="235"/>
-      <c r="N82" s="235"/>
-      <c r="O82" s="235"/>
-      <c r="P82" s="235"/>
+      <c r="M82" s="176"/>
+      <c r="N82" s="176"/>
+      <c r="O82" s="176"/>
+      <c r="P82" s="176"/>
       <c r="Q82" s="171"/>
     </row>
     <row r="83" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6318,12 +6318,12 @@
       <c r="C84" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E84" s="200" t="s">
+      <c r="E84" s="206" t="s">
         <v>82</v>
       </c>
-      <c r="F84" s="200"/>
-      <c r="G84" s="200"/>
-      <c r="H84" s="200"/>
+      <c r="F84" s="206"/>
+      <c r="G84" s="206"/>
+      <c r="H84" s="206"/>
       <c r="L84" s="167"/>
       <c r="M84" s="168"/>
       <c r="N84" s="168"/>
@@ -6332,7 +6332,7 @@
       <c r="Q84" s="169"/>
     </row>
     <row r="85" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="204" t="s">
+      <c r="B85" s="210" t="s">
         <v>85</v>
       </c>
       <c r="C85" s="116"/>
@@ -6354,18 +6354,18 @@
         <v>-</v>
       </c>
       <c r="J85" s="5"/>
-      <c r="L85" s="234" t="str">
+      <c r="L85" s="175" t="str">
         <f>IF(I85=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M85" s="235"/>
-      <c r="N85" s="235"/>
-      <c r="O85" s="235"/>
-      <c r="P85" s="235"/>
+      <c r="M85" s="176"/>
+      <c r="N85" s="176"/>
+      <c r="O85" s="176"/>
+      <c r="P85" s="176"/>
       <c r="Q85" s="171"/>
     </row>
     <row r="86" spans="2:17" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="207"/>
+      <c r="B86" s="213"/>
       <c r="C86" s="119"/>
       <c r="D86" s="119" t="s">
         <v>99</v>
@@ -6385,14 +6385,14 @@
         <v>-</v>
       </c>
       <c r="J86" s="5"/>
-      <c r="L86" s="236" t="str">
+      <c r="L86" s="177" t="str">
         <f>IF(I86=0,"Resulve el empate con 1, o un 2 para indicar el vencedor:","")</f>
         <v/>
       </c>
-      <c r="M86" s="237"/>
-      <c r="N86" s="237"/>
-      <c r="O86" s="237"/>
-      <c r="P86" s="237"/>
+      <c r="M86" s="178"/>
+      <c r="N86" s="178"/>
+      <c r="O86" s="178"/>
+      <c r="P86" s="178"/>
       <c r="Q86" s="172"/>
     </row>
     <row r="87" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6407,12 +6407,12 @@
         <v>38</v>
       </c>
       <c r="D88" s="121"/>
-      <c r="E88" s="200" t="s">
+      <c r="E88" s="206" t="s">
         <v>103</v>
       </c>
-      <c r="F88" s="200"/>
-      <c r="G88" s="200"/>
-      <c r="H88" s="200"/>
+      <c r="F88" s="206"/>
+      <c r="G88" s="206"/>
+      <c r="H88" s="206"/>
       <c r="I88" s="5"/>
       <c r="J88" s="5"/>
     </row>
@@ -6440,12 +6440,12 @@
     <row r="90" spans="2:17" ht="38" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C90" s="121"/>
       <c r="D90" s="121"/>
-      <c r="E90" s="201" t="s">
+      <c r="E90" s="207" t="s">
         <v>83</v>
       </c>
-      <c r="F90" s="201"/>
-      <c r="G90" s="201"/>
-      <c r="H90" s="201"/>
+      <c r="F90" s="207"/>
+      <c r="G90" s="207"/>
+      <c r="H90" s="207"/>
       <c r="I90" s="5"/>
       <c r="J90" s="5"/>
     </row>
@@ -6479,72 +6479,72 @@
       <c r="J93" s="5"/>
     </row>
     <row r="94" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="202" t="s">
+      <c r="B94" s="208" t="s">
         <v>104</v>
       </c>
-      <c r="C94" s="202"/>
-      <c r="D94" s="202"/>
-      <c r="E94" s="202"/>
-      <c r="F94" s="203"/>
-      <c r="G94" s="203"/>
-      <c r="H94" s="203"/>
-      <c r="I94" s="203"/>
-      <c r="J94" s="203"/>
-      <c r="K94" s="203"/>
+      <c r="C94" s="208"/>
+      <c r="D94" s="208"/>
+      <c r="E94" s="208"/>
+      <c r="F94" s="209"/>
+      <c r="G94" s="209"/>
+      <c r="H94" s="209"/>
+      <c r="I94" s="209"/>
+      <c r="J94" s="209"/>
+      <c r="K94" s="209"/>
     </row>
     <row r="95" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="202" t="s">
+      <c r="B95" s="208" t="s">
         <v>105</v>
       </c>
-      <c r="C95" s="202"/>
-      <c r="D95" s="202"/>
-      <c r="E95" s="202"/>
-      <c r="F95" s="203"/>
-      <c r="G95" s="203"/>
-      <c r="H95" s="203"/>
-      <c r="I95" s="203"/>
-      <c r="J95" s="203"/>
-      <c r="K95" s="203"/>
+      <c r="C95" s="208"/>
+      <c r="D95" s="208"/>
+      <c r="E95" s="208"/>
+      <c r="F95" s="209"/>
+      <c r="G95" s="209"/>
+      <c r="H95" s="209"/>
+      <c r="I95" s="209"/>
+      <c r="J95" s="209"/>
+      <c r="K95" s="209"/>
     </row>
     <row r="96" spans="2:17" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="202" t="s">
+      <c r="B96" s="208" t="s">
         <v>106</v>
       </c>
-      <c r="C96" s="202"/>
-      <c r="D96" s="202"/>
-      <c r="E96" s="202"/>
-      <c r="F96" s="203"/>
-      <c r="G96" s="203"/>
-      <c r="H96" s="203"/>
-      <c r="I96" s="203"/>
-      <c r="J96" s="203"/>
-      <c r="K96" s="203"/>
+      <c r="C96" s="208"/>
+      <c r="D96" s="208"/>
+      <c r="E96" s="208"/>
+      <c r="F96" s="209"/>
+      <c r="G96" s="209"/>
+      <c r="H96" s="209"/>
+      <c r="I96" s="209"/>
+      <c r="J96" s="209"/>
+      <c r="K96" s="209"/>
     </row>
     <row r="97" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B97" s="199" t="s">
+      <c r="B97" s="205" t="s">
         <v>107</v>
       </c>
-      <c r="C97" s="199"/>
-      <c r="D97" s="199"/>
-      <c r="E97" s="199"/>
-      <c r="F97" s="199"/>
-      <c r="G97" s="199"/>
-      <c r="H97" s="199"/>
-      <c r="I97" s="199"/>
-      <c r="J97" s="199"/>
-      <c r="K97" s="199"/>
+      <c r="C97" s="205"/>
+      <c r="D97" s="205"/>
+      <c r="E97" s="205"/>
+      <c r="F97" s="205"/>
+      <c r="G97" s="205"/>
+      <c r="H97" s="205"/>
+      <c r="I97" s="205"/>
+      <c r="J97" s="205"/>
+      <c r="K97" s="205"/>
     </row>
     <row r="98" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="199"/>
-      <c r="C98" s="199"/>
-      <c r="D98" s="199"/>
-      <c r="E98" s="199"/>
-      <c r="F98" s="199"/>
-      <c r="G98" s="199"/>
-      <c r="H98" s="199"/>
-      <c r="I98" s="199"/>
-      <c r="J98" s="199"/>
-      <c r="K98" s="199"/>
+      <c r="B98" s="205"/>
+      <c r="C98" s="205"/>
+      <c r="D98" s="205"/>
+      <c r="E98" s="205"/>
+      <c r="F98" s="205"/>
+      <c r="G98" s="205"/>
+      <c r="H98" s="205"/>
+      <c r="I98" s="205"/>
+      <c r="J98" s="205"/>
+      <c r="K98" s="205"/>
     </row>
     <row r="99" spans="2:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I99" s="5" t="str">
@@ -14627,30 +14627,16 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LNRvUeNQVE0bR7R/gRo9r1T1/xAxaSP+mrs49Gg25bt00BkxSjAHGGFDngR/wK3Su0kpcu5i5+vXJfHuCKeqZg==" saltValue="ohXe/5dAU9Alo4FYHlGNag==" spinCount="100000" sheet="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qO3xY28YXJYdNwfiyBgzB97jZUCXIPOYOSI6DH4RohFEqkmFDTpANZbL1OVG/3mPYB2OVy+o5GLH3c4fvWEduA==" saltValue="UvtoSt+WHIs6cYL/o1UD7Q==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="45">
-    <mergeCell ref="L81:P81"/>
-    <mergeCell ref="L82:P82"/>
-    <mergeCell ref="L85:P85"/>
-    <mergeCell ref="L86:P86"/>
-    <mergeCell ref="L74:P74"/>
-    <mergeCell ref="L75:P75"/>
-    <mergeCell ref="L76:P76"/>
-    <mergeCell ref="L79:P79"/>
-    <mergeCell ref="L80:P80"/>
-    <mergeCell ref="L69:P69"/>
-    <mergeCell ref="L70:P70"/>
-    <mergeCell ref="L71:P71"/>
-    <mergeCell ref="L72:P72"/>
-    <mergeCell ref="L73:P73"/>
-    <mergeCell ref="L36:Q36"/>
-    <mergeCell ref="L44:Q44"/>
-    <mergeCell ref="L52:Q52"/>
-    <mergeCell ref="L60:Q60"/>
-    <mergeCell ref="B36:B41"/>
-    <mergeCell ref="B44:B49"/>
-    <mergeCell ref="B52:B57"/>
-    <mergeCell ref="B60:B65"/>
+    <mergeCell ref="L28:Q28"/>
+    <mergeCell ref="L4:Q4"/>
+    <mergeCell ref="B12:B17"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="B20:B25"/>
+    <mergeCell ref="L20:Q20"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="B28:B33"/>
     <mergeCell ref="B97:K98"/>
     <mergeCell ref="E68:H68"/>
     <mergeCell ref="E78:H78"/>
@@ -14666,14 +14652,28 @@
     <mergeCell ref="B79:B82"/>
     <mergeCell ref="B85:B86"/>
     <mergeCell ref="B94:E94"/>
-    <mergeCell ref="L28:Q28"/>
-    <mergeCell ref="L4:Q4"/>
-    <mergeCell ref="B12:B17"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="L20:Q20"/>
-    <mergeCell ref="B4:B9"/>
-    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="L36:Q36"/>
+    <mergeCell ref="L44:Q44"/>
+    <mergeCell ref="L52:Q52"/>
+    <mergeCell ref="L60:Q60"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="B44:B49"/>
+    <mergeCell ref="B52:B57"/>
+    <mergeCell ref="B60:B65"/>
+    <mergeCell ref="L69:P69"/>
+    <mergeCell ref="L70:P70"/>
+    <mergeCell ref="L71:P71"/>
+    <mergeCell ref="L72:P72"/>
+    <mergeCell ref="L73:P73"/>
+    <mergeCell ref="L81:P81"/>
+    <mergeCell ref="L82:P82"/>
+    <mergeCell ref="L85:P85"/>
+    <mergeCell ref="L86:P86"/>
+    <mergeCell ref="L74:P74"/>
+    <mergeCell ref="L75:P75"/>
+    <mergeCell ref="L76:P76"/>
+    <mergeCell ref="L79:P79"/>
+    <mergeCell ref="L80:P80"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:G9">
     <cfRule type="cellIs" dxfId="63" priority="96" stopIfTrue="1" operator="greaterThanOrEqual">

</xml_diff>